<commit_message>
for everyone and fix some word document
</commit_message>
<xml_diff>
--- a/spravka.xlsx
+++ b/spravka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E27BB9-0ABC-4276-88C5-C43F317A597E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31782B79-14D4-41E7-B098-87E4D80C20BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F75D9C89-4306-4059-A3AC-1960751A3C2E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Имя</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>08.00-26/0849</t>
+  </si>
+  <si>
+    <t>09.03.02.</t>
+  </si>
+  <si>
+    <t>09.04.02.</t>
+  </si>
+  <si>
+    <t>09.03.03.</t>
+  </si>
+  <si>
+    <t>09.02.02.</t>
   </si>
 </sst>
 </file>
@@ -164,10 +176,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -484,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164A3272-4D3A-4434-BCD8-DCDA03CAD440}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +536,7 @@
       <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H1" t="s">
@@ -561,6 +574,9 @@
       <c r="F2" t="s">
         <v>19</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
@@ -596,6 +612,9 @@
       <c r="F3" t="s">
         <v>19</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
@@ -631,6 +650,9 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="H4" s="2" t="s">
         <v>21</v>
       </c>
@@ -666,6 +688,9 @@
       <c r="F5" t="s">
         <v>20</v>
       </c>
+      <c r="G5" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
@@ -700,6 +725,9 @@
       </c>
       <c r="F6" t="s">
         <v>19</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>22</v>

</xml_diff>